<commit_message>
working upload for the data base and site,person and site param teble
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trotsiuv/Documents/work/projects/2018 fonti xcell/xcell_db/db_create/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{06055CA2-B565-4645-8BF7-C4AF22BF0232}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F8FD9B72-514A-6F49-AFD6-CC5AF64DB018}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="1080" windowWidth="27560" windowHeight="16280" tabRatio="815" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1780" yWindow="1020" windowWidth="27560" windowHeight="16280" tabRatio="815" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="country_fk" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3132" uniqueCount="2935">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="2941">
   <si>
     <t>Afganistan</t>
   </si>
@@ -8929,6 +8929,24 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>aspect</t>
+  </si>
+  <si>
+    <t>degrees</t>
+  </si>
+  <si>
+    <t>aspect of the site location</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>slope of the site</t>
+  </si>
+  <si>
+    <t>percentage</t>
   </si>
 </sst>
 </file>
@@ -12289,7 +12307,7 @@
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -21634,10 +21652,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21758,8 +21776,32 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>2935</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>2936</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2937</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2938</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2940</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2939</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
upload roxas done up to subsample
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="country_fk" sheetId="1" r:id="rId1"/>
@@ -8690,9 +8690,6 @@
     <t>double cell wall thickness on the radial direction (radial file)</t>
   </si>
   <si>
-    <t>band-width</t>
-  </si>
-  <si>
     <t>"Y" if only EW has been measured (e.g. for vessels in ring-porous species)</t>
   </si>
   <si>
@@ -8941,6 +8938,9 @@
   </si>
   <si>
     <t>2cwtrad</t>
+  </si>
+  <si>
+    <t>band_width</t>
   </si>
 </sst>
 </file>
@@ -9805,7 +9805,7 @@
         <v>506</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12100,8 +12100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12112,7 +12112,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2808</v>
@@ -12146,7 +12146,7 @@
         <v>2805</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>2822</v>
@@ -12160,7 +12160,7 @@
         <v>2809</v>
       </c>
       <c r="C4" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="D4" t="s">
         <v>2815</v>
@@ -12174,7 +12174,7 @@
         <v>2810</v>
       </c>
       <c r="C5" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="D5" t="s">
         <v>2821</v>
@@ -12185,7 +12185,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="C6" t="s">
         <v>2756</v>
@@ -12202,10 +12202,10 @@
         <v>2811</v>
       </c>
       <c r="C7" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="D7" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12216,7 +12216,7 @@
         <v>2812</v>
       </c>
       <c r="C8" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D8" t="s">
         <v>2817</v>
@@ -12230,7 +12230,7 @@
         <v>2813</v>
       </c>
       <c r="C9" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D9" t="s">
         <v>2818</v>
@@ -12244,7 +12244,7 @@
         <v>2814</v>
       </c>
       <c r="C10" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D10" t="s">
         <v>2819</v>
@@ -12269,13 +12269,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>2881</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2917</v>
+      </c>
+      <c r="D12" t="s">
         <v>2882</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2918</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2883</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -12283,13 +12283,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2864</v>
+        <v>2940</v>
       </c>
       <c r="C13" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="D13" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
     </row>
   </sheetData>
@@ -12311,7 +12311,7 @@
   </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -12322,7 +12322,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2808</v>
@@ -12373,7 +12373,7 @@
         <v>2754</v>
       </c>
       <c r="D4" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12387,7 +12387,7 @@
         <v>2754</v>
       </c>
       <c r="D5" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12401,7 +12401,7 @@
         <v>2756</v>
       </c>
       <c r="D6" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12415,7 +12415,7 @@
         <v>2756</v>
       </c>
       <c r="D7" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12429,7 +12429,7 @@
         <v>2756</v>
       </c>
       <c r="D8" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12443,7 +12443,7 @@
         <v>2756</v>
       </c>
       <c r="D9" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12639,7 +12639,7 @@
         <v>2754</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -12653,7 +12653,7 @@
         <v>2754</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -12793,7 +12793,7 @@
         <v>2755</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -12857,7 +12857,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="C39" t="s">
         <v>2754</v>
@@ -12877,7 +12877,7 @@
         <v>2756</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -12891,7 +12891,7 @@
         <v>2756</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -12905,7 +12905,7 @@
         <v>2755</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -12933,7 +12933,7 @@
         <v>2756</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -12947,7 +12947,7 @@
         <v>2756</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -12961,7 +12961,7 @@
         <v>2756</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -13045,7 +13045,7 @@
         <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2583</v>
@@ -13491,7 +13491,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="7" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="B41" t="s">
         <v>651</v>
@@ -14717,7 +14717,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="7" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="B153" t="s">
         <v>874</v>
@@ -14978,7 +14978,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="7" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="B177" t="s">
         <v>922</v>
@@ -15481,7 +15481,7 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="7" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="B226" t="s">
         <v>1018</v>
@@ -15771,7 +15771,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="7" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="B251" t="s">
         <v>1066</v>
@@ -18367,7 +18367,7 @@
     </row>
     <row r="487" spans="1:3">
       <c r="A487" s="7" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="B487" t="s">
         <v>1533</v>
@@ -18378,7 +18378,7 @@
     </row>
     <row r="488" spans="1:3">
       <c r="A488" s="7" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="B488" t="s">
         <v>1535</v>
@@ -18411,7 +18411,7 @@
     </row>
     <row r="491" spans="1:3">
       <c r="A491" s="7" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="B491" t="s">
         <v>1541</v>
@@ -18983,7 +18983,7 @@
     </row>
     <row r="546" spans="1:3">
       <c r="A546" s="7" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="B546" t="s">
         <v>1648</v>
@@ -19950,7 +19950,7 @@
     </row>
     <row r="635" spans="1:3">
       <c r="A635" s="7" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="B635" t="s">
         <v>1824</v>
@@ -20158,7 +20158,7 @@
     </row>
     <row r="655" spans="1:3">
       <c r="A655" s="7" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B655" t="s">
         <v>1863</v>
@@ -20765,7 +20765,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>511</v>
@@ -20832,7 +20832,7 @@
         <v>528</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>506</v>
@@ -21669,7 +21669,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2808</v>
@@ -21689,10 +21689,10 @@
         <v>545</v>
       </c>
       <c r="C2" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D2" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21706,7 +21706,7 @@
         <v>2756</v>
       </c>
       <c r="D3" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21720,7 +21720,7 @@
         <v>2756</v>
       </c>
       <c r="D4" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21734,7 +21734,7 @@
         <v>2756</v>
       </c>
       <c r="D5" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -21745,10 +21745,10 @@
         <v>2827</v>
       </c>
       <c r="C6" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D6" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -21759,10 +21759,10 @@
         <v>2826</v>
       </c>
       <c r="C7" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D7" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -21773,10 +21773,10 @@
         <v>2825</v>
       </c>
       <c r="C8" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D8" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -21784,13 +21784,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>2918</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>2919</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" t="s">
         <v>2920</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2921</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -21798,13 +21798,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>2921</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2923</v>
+      </c>
+      <c r="D10" t="s">
         <v>2922</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2924</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2923</v>
       </c>
     </row>
   </sheetData>
@@ -21830,7 +21830,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2808</v>
@@ -21853,7 +21853,7 @@
         <v>2756</v>
       </c>
       <c r="D2" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21864,10 +21864,10 @@
         <v>2828</v>
       </c>
       <c r="C3" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D3" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21878,10 +21878,10 @@
         <v>2829</v>
       </c>
       <c r="C4" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="D4" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21892,10 +21892,10 @@
         <v>2830</v>
       </c>
       <c r="C5" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="D5" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
     </row>
   </sheetData>
@@ -21926,7 +21926,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2808</v>
@@ -21943,13 +21943,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>2756</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="26" customFormat="1">
@@ -21963,7 +21963,7 @@
         <v>2756</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21974,10 +21974,10 @@
         <v>2831</v>
       </c>
       <c r="C4" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="D4" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21988,10 +21988,10 @@
         <v>2832</v>
       </c>
       <c r="C5" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="D5" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="26" customFormat="1">
@@ -22002,10 +22002,10 @@
         <v>2850</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
     </row>
   </sheetData>
@@ -22038,10 +22038,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2793</v>
@@ -22056,7 +22056,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C2" t="s">
         <v>2796</v>
@@ -22070,7 +22070,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C3" t="s">
         <v>2796</v>
@@ -22084,7 +22084,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C4" t="s">
         <v>2796</v>
@@ -22098,13 +22098,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C5" t="s">
         <v>2796</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -22112,7 +22112,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C6" t="s">
         <v>2796</v>
@@ -22126,7 +22126,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C7" t="s">
         <v>2796</v>
@@ -22155,7 +22155,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="C9" t="s">
         <v>2796</v>
@@ -22169,7 +22169,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="C10" t="s">
         <v>2796</v>
@@ -22183,7 +22183,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="C11" t="s">
         <v>2796</v>
@@ -22197,7 +22197,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="C12" t="s">
         <v>2796</v>
@@ -22211,10 +22211,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C13" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="D13" t="s">
         <v>2798</v>
@@ -22226,10 +22226,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C14" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>2799</v>
@@ -22241,7 +22241,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C15" t="s">
         <v>2796</v>

</xml_diff>

<commit_message>
finishing script up-load Roxas
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="country_fk" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="2941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3141" uniqueCount="2942">
   <si>
     <t>Afganistan</t>
   </si>
@@ -8199,9 +8199,6 @@
   </si>
   <si>
     <t>dist</t>
-  </si>
-  <si>
-    <t>lum</t>
   </si>
   <si>
     <t>drad</t>
@@ -8941,6 +8938,12 @@
   </si>
   <si>
     <t>band_width</t>
+  </si>
+  <si>
+    <t>bend</t>
+  </si>
+  <si>
+    <t>la</t>
   </si>
 </sst>
 </file>
@@ -9088,12 +9091,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9269,7 +9277,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="138">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -9401,6 +9409,11 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -9805,7 +9818,7 @@
         <v>506</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12100,7 +12113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -12112,10 +12125,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -12129,13 +12142,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2823</v>
+        <v>2822</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="26" customFormat="1">
@@ -12143,13 +12156,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>2822</v>
+        <v>2821</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -12157,13 +12170,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="C4" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="D4" t="s">
-        <v>2815</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12171,13 +12184,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="C5" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="D5" t="s">
-        <v>2821</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12185,13 +12198,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2880</v>
+        <v>2879</v>
       </c>
       <c r="C6" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D6" t="s">
-        <v>2820</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12199,13 +12212,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="C7" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="D7" t="s">
-        <v>2864</v>
+        <v>2863</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12213,13 +12226,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="C8" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D8" t="s">
-        <v>2817</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12227,13 +12240,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="C9" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D9" t="s">
-        <v>2818</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12241,13 +12254,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="C10" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D10" t="s">
-        <v>2819</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -12258,10 +12271,10 @@
         <v>520</v>
       </c>
       <c r="C11" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D11" t="s">
-        <v>2816</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -12269,13 +12282,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>2880</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2916</v>
+      </c>
+      <c r="D12" t="s">
         <v>2881</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2917</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2882</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -12283,13 +12296,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2940</v>
+        <v>2939</v>
       </c>
       <c r="C13" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="D13" t="s">
-        <v>2878</v>
+        <v>2877</v>
       </c>
     </row>
   </sheetData>
@@ -12309,10 +12322,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -12322,10 +12335,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -12339,13 +12352,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>2778</v>
+        <v>2777</v>
       </c>
       <c r="C2" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>2781</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -12353,13 +12366,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>2778</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>2791</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>2779</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>2792</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>2780</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -12367,13 +12380,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="C4" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D4" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12381,13 +12394,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>2770</v>
+        <v>2769</v>
       </c>
       <c r="C5" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D5" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12395,13 +12408,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>2771</v>
+        <v>2770</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D6" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12409,13 +12422,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>2772</v>
+        <v>2771</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D7" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12423,13 +12436,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>2773</v>
+        <v>2772</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D8" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12437,13 +12450,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>2774</v>
+        <v>2773</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D9" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12451,13 +12464,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>2775</v>
+        <v>2774</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>2782</v>
+        <v>2781</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -12465,13 +12478,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>2776</v>
+        <v>2775</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>2783</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -12479,13 +12492,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>2777</v>
+        <v>2776</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>2784</v>
+        <v>2783</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -12493,13 +12506,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>2785</v>
+        <v>2784</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -12507,13 +12520,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="C14" t="s">
-        <v>2861</v>
+        <v>2860</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>2786</v>
+        <v>2785</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -12521,13 +12534,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>2854</v>
+        <v>2853</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>2792</v>
+        <v>2791</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>2787</v>
+        <v>2786</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -12535,13 +12548,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>2788</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -12552,10 +12565,10 @@
         <v>2716</v>
       </c>
       <c r="C17" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>2752</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -12566,10 +12579,10 @@
         <v>2717</v>
       </c>
       <c r="C18" t="s">
-        <v>2758</v>
+        <v>2757</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>2751</v>
+        <v>2750</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -12580,10 +12593,10 @@
         <v>2718</v>
       </c>
       <c r="C19" t="s">
-        <v>2759</v>
+        <v>2758</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>2750</v>
+        <v>2749</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -12594,10 +12607,10 @@
         <v>2719</v>
       </c>
       <c r="C20" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>2753</v>
+        <v>2752</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -12608,10 +12621,10 @@
         <v>2720</v>
       </c>
       <c r="C21" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>2748</v>
+        <v>2747</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -12619,13 +12632,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>2760</v>
+        <v>2759</v>
       </c>
       <c r="C22" t="s">
-        <v>2757</v>
+        <v>2756</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>2749</v>
+        <v>2748</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -12633,13 +12646,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="C23" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -12647,13 +12660,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="C24" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>2932</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -12661,13 +12674,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>2724</v>
+        <v>2723</v>
       </c>
       <c r="C25" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>2767</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -12675,13 +12688,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>2725</v>
+        <v>2724</v>
       </c>
       <c r="C26" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>2768</v>
+        <v>2767</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -12689,13 +12702,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>2726</v>
+        <v>2725</v>
       </c>
       <c r="C27" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>2735</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -12703,13 +12716,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>2727</v>
+        <v>2726</v>
       </c>
       <c r="C28" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>2736</v>
+        <v>2735</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -12717,13 +12730,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>2728</v>
+        <v>2727</v>
       </c>
       <c r="C29" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>2737</v>
+        <v>2736</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -12731,13 +12744,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>2729</v>
+        <v>2728</v>
       </c>
       <c r="C30" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>2738</v>
+        <v>2737</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -12745,13 +12758,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>2730</v>
+        <v>2729</v>
       </c>
       <c r="C31" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>2739</v>
+        <v>2738</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -12759,13 +12772,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>2731</v>
+        <v>2730</v>
       </c>
       <c r="C32" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>2740</v>
+        <v>2739</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -12773,13 +12786,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>2746</v>
+        <v>2745</v>
       </c>
       <c r="C33" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>2741</v>
+        <v>2740</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -12787,13 +12800,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>2721</v>
+        <v>2941</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -12801,13 +12814,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>2761</v>
+        <v>2760</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>2742</v>
+        <v>2741</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -12815,13 +12828,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>2762</v>
+        <v>2761</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>2743</v>
+        <v>2742</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -12829,13 +12842,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>2747</v>
+        <v>2746</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>2744</v>
+        <v>2743</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -12843,13 +12856,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>2732</v>
+        <v>2731</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>2849</v>
+        <v>2848</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -12857,13 +12870,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="C39" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>2863</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -12871,13 +12884,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>2733</v>
+        <v>2732</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>2933</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -12885,13 +12898,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>2734</v>
+        <v>2733</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -12899,13 +12912,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>2851</v>
+        <v>2850</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>2755</v>
+        <v>2754</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -12913,13 +12926,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>2763</v>
+        <v>2762</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>2745</v>
+        <v>2744</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -12927,13 +12940,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>2764</v>
+        <v>2763</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -12941,13 +12954,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>2765</v>
+        <v>2764</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -12955,13 +12968,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>2766</v>
+        <v>2765</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -12969,13 +12982,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="C47" t="s">
-        <v>2859</v>
+        <v>2858</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>2790</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -12983,13 +12996,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="C48" t="s">
-        <v>2860</v>
+        <v>2859</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>2791</v>
+        <v>2790</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -12997,13 +13010,27 @@
         <v>48</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="C49" t="s">
-        <v>2754</v>
+        <v>2753</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>2789</v>
+        <v>2788</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>2940</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2755</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>2743</v>
       </c>
     </row>
   </sheetData>
@@ -13045,7 +13072,7 @@
         <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2583</v>
@@ -13491,7 +13518,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="7" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="B41" t="s">
         <v>651</v>
@@ -14717,7 +14744,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="7" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="B153" t="s">
         <v>874</v>
@@ -14978,7 +15005,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="7" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="B177" t="s">
         <v>922</v>
@@ -15481,7 +15508,7 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="7" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="B226" t="s">
         <v>1018</v>
@@ -15771,7 +15798,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="7" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="B251" t="s">
         <v>1066</v>
@@ -18367,7 +18394,7 @@
     </row>
     <row r="487" spans="1:3">
       <c r="A487" s="7" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="B487" t="s">
         <v>1533</v>
@@ -18378,7 +18405,7 @@
     </row>
     <row r="488" spans="1:3">
       <c r="A488" s="7" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="B488" t="s">
         <v>1535</v>
@@ -18411,7 +18438,7 @@
     </row>
     <row r="491" spans="1:3">
       <c r="A491" s="7" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="B491" t="s">
         <v>1541</v>
@@ -18983,7 +19010,7 @@
     </row>
     <row r="546" spans="1:3">
       <c r="A546" s="7" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="B546" t="s">
         <v>1648</v>
@@ -19950,7 +19977,7 @@
     </row>
     <row r="635" spans="1:3">
       <c r="A635" s="7" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="B635" t="s">
         <v>1824</v>
@@ -20158,7 +20185,7 @@
     </row>
     <row r="655" spans="1:3">
       <c r="A655" s="7" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="B655" t="s">
         <v>1863</v>
@@ -20765,7 +20792,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>511</v>
@@ -20832,7 +20859,7 @@
         <v>528</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2879</v>
+        <v>2878</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>506</v>
@@ -20935,7 +20962,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>2835</v>
+        <v>2834</v>
       </c>
       <c r="B6" t="s">
         <v>551</v>
@@ -20981,7 +21008,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>2836</v>
+        <v>2835</v>
       </c>
       <c r="B8" t="s">
         <v>567</v>
@@ -21041,7 +21068,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="B11" t="s">
         <v>2595</v>
@@ -21095,7 +21122,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>2837</v>
+        <v>2836</v>
       </c>
       <c r="B14" t="s">
         <v>2598</v>
@@ -21112,7 +21139,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>2838</v>
+        <v>2837</v>
       </c>
       <c r="B15" t="s">
         <v>2599</v>
@@ -21129,7 +21156,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>2839</v>
+        <v>2838</v>
       </c>
       <c r="B16" t="s">
         <v>2600</v>
@@ -21169,7 +21196,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>2840</v>
+        <v>2839</v>
       </c>
       <c r="B18" t="s">
         <v>2639</v>
@@ -21240,7 +21267,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>2841</v>
+        <v>2840</v>
       </c>
       <c r="B22" t="s">
         <v>2709</v>
@@ -21283,7 +21310,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="B24" t="s">
         <v>2649</v>
@@ -21329,7 +21356,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="B26" t="s">
         <v>2663</v>
@@ -21349,7 +21376,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>2844</v>
+        <v>2843</v>
       </c>
       <c r="B27" t="s">
         <v>2667</v>
@@ -21372,7 +21399,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>2845</v>
+        <v>2844</v>
       </c>
       <c r="B28" t="s">
         <v>2670</v>
@@ -21418,7 +21445,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>2846</v>
+        <v>2845</v>
       </c>
       <c r="B30" t="s">
         <v>2679</v>
@@ -21498,7 +21525,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>2847</v>
+        <v>2846</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>2698</v>
@@ -21561,7 +21588,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>2848</v>
+        <v>2847</v>
       </c>
       <c r="B37" t="s">
         <v>2711</v>
@@ -21669,10 +21696,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -21689,10 +21716,10 @@
         <v>545</v>
       </c>
       <c r="C2" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="D2" t="s">
-        <v>2883</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21703,10 +21730,10 @@
         <v>546</v>
       </c>
       <c r="C3" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D3" t="s">
-        <v>2884</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21717,10 +21744,10 @@
         <v>547</v>
       </c>
       <c r="C4" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D4" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21731,10 +21758,10 @@
         <v>548</v>
       </c>
       <c r="C5" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D5" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -21742,13 +21769,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2827</v>
+        <v>2826</v>
       </c>
       <c r="C6" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D6" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -21756,13 +21783,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2826</v>
+        <v>2825</v>
       </c>
       <c r="C7" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D7" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -21770,13 +21797,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2825</v>
+        <v>2824</v>
       </c>
       <c r="C8" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="D8" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -21784,13 +21811,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>2917</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>2918</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" t="s">
         <v>2919</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2920</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -21798,13 +21825,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>2920</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2922</v>
+      </c>
+      <c r="D10" t="s">
         <v>2921</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2923</v>
-      </c>
-      <c r="D10" t="s">
-        <v>2922</v>
       </c>
     </row>
   </sheetData>
@@ -21830,10 +21857,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -21847,13 +21874,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="C2" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D2" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21861,13 +21888,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2828</v>
+        <v>2827</v>
       </c>
       <c r="C3" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="D3" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21875,13 +21902,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2829</v>
+        <v>2828</v>
       </c>
       <c r="C4" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D4" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21889,13 +21916,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2830</v>
+        <v>2829</v>
       </c>
       <c r="C5" t="s">
-        <v>2911</v>
+        <v>2910</v>
       </c>
       <c r="D5" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
   </sheetData>
@@ -21926,10 +21953,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2715</v>
@@ -21943,13 +21970,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2876</v>
+        <v>2875</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="26" customFormat="1">
@@ -21957,13 +21984,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>2824</v>
+        <v>2823</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>2756</v>
+        <v>2755</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>2873</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21971,13 +21998,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2831</v>
+        <v>2830</v>
       </c>
       <c r="C4" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D4" t="s">
-        <v>2874</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21985,13 +22012,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="C5" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="D5" t="s">
-        <v>2875</v>
+        <v>2874</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="26" customFormat="1">
@@ -21999,13 +22026,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>2850</v>
+        <v>2849</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>2877</v>
+        <v>2876</v>
       </c>
     </row>
   </sheetData>
@@ -22038,13 +22065,13 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2865</v>
+        <v>2864</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2793</v>
+        <v>2792</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>521</v>
@@ -22056,10 +22083,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="C2" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>522</v>
@@ -22070,10 +22097,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="C3" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>523</v>
@@ -22084,10 +22111,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="C4" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>524</v>
@@ -22098,13 +22125,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="C5" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>2870</v>
+        <v>2869</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -22112,10 +22139,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C6" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>526</v>
@@ -22126,13 +22153,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2867</v>
+        <v>2866</v>
       </c>
       <c r="C7" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>2807</v>
+        <v>2806</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -22140,10 +22167,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="C8" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>571</v>
@@ -22155,10 +22182,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C9" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>522</v>
@@ -22169,10 +22196,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C10" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>523</v>
@@ -22183,10 +22210,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C11" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>524</v>
@@ -22197,10 +22224,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2868</v>
+        <v>2867</v>
       </c>
       <c r="C12" t="s">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>525</v>
@@ -22211,13 +22238,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="C13" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="D13" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
       <c r="F13" s="20"/>
     </row>
@@ -22226,13 +22253,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="C14" t="s">
-        <v>2869</v>
+        <v>2868</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>2799</v>
+        <v>2798</v>
       </c>
       <c r="F14" s="16"/>
     </row>
@@ -22241,13 +22268,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>2871</v>
+        <v>2870</v>
       </c>
       <c r="C15" t="s">
+        <v>2795</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>2796</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>2797</v>
       </c>
       <c r="F15" s="16"/>
     </row>
@@ -22256,13 +22283,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="C16" t="s">
-        <v>2800</v>
+        <v>2799</v>
       </c>
       <c r="D16" t="s">
-        <v>2798</v>
+        <v>2797</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -22270,13 +22297,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="C17" t="s">
+        <v>2800</v>
+      </c>
+      <c r="D17" t="s">
         <v>2801</v>
-      </c>
-      <c r="D17" t="s">
-        <v>2802</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -22284,13 +22311,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>2795</v>
+        <v>2794</v>
       </c>
       <c r="C18" t="s">
+        <v>2802</v>
+      </c>
+      <c r="D18" t="s">
         <v>2803</v>
-      </c>
-      <c r="D18" t="s">
-        <v>2804</v>
       </c>
     </row>
     <row r="19" spans="1:4">

</xml_diff>

<commit_message>
adjustment of error found when uploading second site
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="815" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="country_fk" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3141" uniqueCount="2942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="2942">
   <si>
     <t>Afganistan</t>
   </si>
@@ -8455,13 +8455,7 @@
     <t>hardware</t>
   </si>
   <si>
-    <t>anatomy</t>
-  </si>
-  <si>
     <t>Radiodensitometry</t>
-  </si>
-  <si>
-    <t>photography</t>
   </si>
   <si>
     <t>Lignovision</t>
@@ -8944,6 +8938,12 @@
   </si>
   <si>
     <t>la</t>
+  </si>
+  <si>
+    <t>light microscope</t>
+  </si>
+  <si>
+    <t>confocal microscope</t>
   </si>
 </sst>
 </file>
@@ -9091,12 +9091,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="138">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9277,7 +9284,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="138">
+  <cellStyles count="145">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -9414,6 +9421,13 @@
     <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -9818,7 +9832,7 @@
         <v>506</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2893</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -12125,10 +12139,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -12142,13 +12156,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>2805</v>
+        <v>2803</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>2755</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2822</v>
+        <v>2820</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="26" customFormat="1">
@@ -12156,13 +12170,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>2804</v>
+        <v>2802</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>2912</v>
+        <v>2910</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>2821</v>
+        <v>2819</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -12170,13 +12184,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2808</v>
+        <v>2806</v>
       </c>
       <c r="C4" t="s">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="D4" t="s">
-        <v>2814</v>
+        <v>2812</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12184,13 +12198,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2809</v>
+        <v>2807</v>
       </c>
       <c r="C5" t="s">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="D5" t="s">
-        <v>2820</v>
+        <v>2818</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12198,13 +12212,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2879</v>
+        <v>2877</v>
       </c>
       <c r="C6" t="s">
         <v>2755</v>
       </c>
       <c r="D6" t="s">
-        <v>2819</v>
+        <v>2817</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12212,13 +12226,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2810</v>
+        <v>2808</v>
       </c>
       <c r="C7" t="s">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="D7" t="s">
-        <v>2863</v>
+        <v>2861</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12226,13 +12240,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2811</v>
+        <v>2809</v>
       </c>
       <c r="C8" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D8" t="s">
-        <v>2816</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12240,13 +12254,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2812</v>
+        <v>2810</v>
       </c>
       <c r="C9" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D9" t="s">
-        <v>2817</v>
+        <v>2815</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12254,13 +12268,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2813</v>
+        <v>2811</v>
       </c>
       <c r="C10" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D10" t="s">
-        <v>2818</v>
+        <v>2816</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -12274,7 +12288,7 @@
         <v>2755</v>
       </c>
       <c r="D11" t="s">
-        <v>2815</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -12282,13 +12296,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2880</v>
+        <v>2878</v>
       </c>
       <c r="C12" t="s">
-        <v>2916</v>
+        <v>2914</v>
       </c>
       <c r="D12" t="s">
-        <v>2881</v>
+        <v>2879</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -12296,13 +12310,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2939</v>
+        <v>2937</v>
       </c>
       <c r="C13" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="D13" t="s">
-        <v>2877</v>
+        <v>2875</v>
       </c>
     </row>
   </sheetData>
@@ -12324,7 +12338,7 @@
   </sheetPr>
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -12335,10 +12349,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -12386,7 +12400,7 @@
         <v>2753</v>
       </c>
       <c r="D4" t="s">
-        <v>2923</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -12400,7 +12414,7 @@
         <v>2753</v>
       </c>
       <c r="D5" t="s">
-        <v>2924</v>
+        <v>2922</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -12414,7 +12428,7 @@
         <v>2755</v>
       </c>
       <c r="D6" t="s">
-        <v>2925</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -12428,7 +12442,7 @@
         <v>2755</v>
       </c>
       <c r="D7" t="s">
-        <v>2926</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -12442,7 +12456,7 @@
         <v>2755</v>
       </c>
       <c r="D8" t="s">
-        <v>2927</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -12456,7 +12470,7 @@
         <v>2755</v>
       </c>
       <c r="D9" t="s">
-        <v>2928</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -12506,7 +12520,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>2851</v>
+        <v>2849</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>2758</v>
@@ -12520,10 +12534,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>2852</v>
+        <v>2850</v>
       </c>
       <c r="C14" t="s">
-        <v>2860</v>
+        <v>2858</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>2785</v>
@@ -12534,7 +12548,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>2791</v>
@@ -12548,10 +12562,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>2854</v>
+        <v>2852</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>2861</v>
+        <v>2859</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>2787</v>
@@ -12652,7 +12666,7 @@
         <v>2753</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>2930</v>
+        <v>2928</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -12666,7 +12680,7 @@
         <v>2753</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>2931</v>
+        <v>2929</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -12800,13 +12814,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>2754</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>2929</v>
+        <v>2927</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -12862,7 +12876,7 @@
         <v>2754</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>2848</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -12870,13 +12884,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>2938</v>
+        <v>2936</v>
       </c>
       <c r="C39" t="s">
         <v>2753</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>2862</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -12890,7 +12904,7 @@
         <v>2755</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>2932</v>
+        <v>2930</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -12904,7 +12918,7 @@
         <v>2755</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>2933</v>
+        <v>2931</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -12912,13 +12926,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>2850</v>
+        <v>2848</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>2754</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>2934</v>
+        <v>2932</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -12946,7 +12960,7 @@
         <v>2755</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>2935</v>
+        <v>2933</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -12960,7 +12974,7 @@
         <v>2755</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>2936</v>
+        <v>2934</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -12974,7 +12988,7 @@
         <v>2755</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>2937</v>
+        <v>2935</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -12982,10 +12996,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>2855</v>
+        <v>2853</v>
       </c>
       <c r="C47" t="s">
-        <v>2858</v>
+        <v>2856</v>
       </c>
       <c r="D47" s="17" t="s">
         <v>2789</v>
@@ -12996,10 +13010,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>2856</v>
+        <v>2854</v>
       </c>
       <c r="C48" t="s">
-        <v>2859</v>
+        <v>2857</v>
       </c>
       <c r="D48" s="17" t="s">
         <v>2790</v>
@@ -13010,7 +13024,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>2857</v>
+        <v>2855</v>
       </c>
       <c r="C49" t="s">
         <v>2753</v>
@@ -13024,7 +13038,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>2940</v>
+        <v>2938</v>
       </c>
       <c r="C50" t="s">
         <v>2755</v>
@@ -13072,7 +13086,7 @@
         <v>508</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2894</v>
+        <v>2892</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2583</v>
@@ -13518,7 +13532,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="7" t="s">
-        <v>2895</v>
+        <v>2893</v>
       </c>
       <c r="B41" t="s">
         <v>651</v>
@@ -14744,7 +14758,7 @@
     </row>
     <row r="153" spans="1:6">
       <c r="A153" s="7" t="s">
-        <v>2896</v>
+        <v>2894</v>
       </c>
       <c r="B153" t="s">
         <v>874</v>
@@ -15005,7 +15019,7 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="7" t="s">
-        <v>2897</v>
+        <v>2895</v>
       </c>
       <c r="B177" t="s">
         <v>922</v>
@@ -15508,7 +15522,7 @@
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="7" t="s">
-        <v>2898</v>
+        <v>2896</v>
       </c>
       <c r="B226" t="s">
         <v>1018</v>
@@ -15798,7 +15812,7 @@
     </row>
     <row r="251" spans="1:6">
       <c r="A251" s="7" t="s">
-        <v>2899</v>
+        <v>2897</v>
       </c>
       <c r="B251" t="s">
         <v>1066</v>
@@ -18394,7 +18408,7 @@
     </row>
     <row r="487" spans="1:3">
       <c r="A487" s="7" t="s">
-        <v>2901</v>
+        <v>2899</v>
       </c>
       <c r="B487" t="s">
         <v>1533</v>
@@ -18405,7 +18419,7 @@
     </row>
     <row r="488" spans="1:3">
       <c r="A488" s="7" t="s">
-        <v>2902</v>
+        <v>2900</v>
       </c>
       <c r="B488" t="s">
         <v>1535</v>
@@ -18438,7 +18452,7 @@
     </row>
     <row r="491" spans="1:3">
       <c r="A491" s="7" t="s">
-        <v>2900</v>
+        <v>2898</v>
       </c>
       <c r="B491" t="s">
         <v>1541</v>
@@ -19010,7 +19024,7 @@
     </row>
     <row r="546" spans="1:3">
       <c r="A546" s="7" t="s">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="B546" t="s">
         <v>1648</v>
@@ -19977,7 +19991,7 @@
     </row>
     <row r="635" spans="1:3">
       <c r="A635" s="7" t="s">
-        <v>2904</v>
+        <v>2902</v>
       </c>
       <c r="B635" t="s">
         <v>1824</v>
@@ -20185,7 +20199,7 @@
     </row>
     <row r="655" spans="1:3">
       <c r="A655" s="7" t="s">
-        <v>2905</v>
+        <v>2903</v>
       </c>
       <c r="B655" t="s">
         <v>1863</v>
@@ -20792,7 +20806,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>511</v>
@@ -20859,7 +20873,7 @@
         <v>528</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2878</v>
+        <v>2876</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>506</v>
@@ -20962,7 +20976,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>2834</v>
+        <v>2832</v>
       </c>
       <c r="B6" t="s">
         <v>551</v>
@@ -21008,7 +21022,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>2835</v>
+        <v>2833</v>
       </c>
       <c r="B8" t="s">
         <v>567</v>
@@ -21068,7 +21082,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>2833</v>
+        <v>2831</v>
       </c>
       <c r="B11" t="s">
         <v>2595</v>
@@ -21122,7 +21136,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>2836</v>
+        <v>2834</v>
       </c>
       <c r="B14" t="s">
         <v>2598</v>
@@ -21139,7 +21153,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>2837</v>
+        <v>2835</v>
       </c>
       <c r="B15" t="s">
         <v>2599</v>
@@ -21156,7 +21170,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>2838</v>
+        <v>2836</v>
       </c>
       <c r="B16" t="s">
         <v>2600</v>
@@ -21196,7 +21210,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>2839</v>
+        <v>2837</v>
       </c>
       <c r="B18" t="s">
         <v>2639</v>
@@ -21267,7 +21281,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>2840</v>
+        <v>2838</v>
       </c>
       <c r="B22" t="s">
         <v>2709</v>
@@ -21310,7 +21324,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>2841</v>
+        <v>2839</v>
       </c>
       <c r="B24" t="s">
         <v>2649</v>
@@ -21356,7 +21370,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>2842</v>
+        <v>2840</v>
       </c>
       <c r="B26" t="s">
         <v>2663</v>
@@ -21376,7 +21390,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>2843</v>
+        <v>2841</v>
       </c>
       <c r="B27" t="s">
         <v>2667</v>
@@ -21399,7 +21413,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>2844</v>
+        <v>2842</v>
       </c>
       <c r="B28" t="s">
         <v>2670</v>
@@ -21445,7 +21459,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>2845</v>
+        <v>2843</v>
       </c>
       <c r="B30" t="s">
         <v>2679</v>
@@ -21525,7 +21539,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>2846</v>
+        <v>2844</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>2698</v>
@@ -21588,7 +21602,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>2847</v>
+        <v>2845</v>
       </c>
       <c r="B37" t="s">
         <v>2711</v>
@@ -21696,10 +21710,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -21716,10 +21730,10 @@
         <v>545</v>
       </c>
       <c r="C2" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="D2" t="s">
-        <v>2882</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21733,7 +21747,7 @@
         <v>2755</v>
       </c>
       <c r="D3" t="s">
-        <v>2883</v>
+        <v>2881</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21747,7 +21761,7 @@
         <v>2755</v>
       </c>
       <c r="D4" t="s">
-        <v>2884</v>
+        <v>2882</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21761,7 +21775,7 @@
         <v>2755</v>
       </c>
       <c r="D5" t="s">
-        <v>2885</v>
+        <v>2883</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -21769,13 +21783,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2826</v>
+        <v>2824</v>
       </c>
       <c r="C6" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D6" t="s">
-        <v>2886</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -21783,13 +21797,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="C7" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D7" t="s">
-        <v>2887</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -21797,13 +21811,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2824</v>
+        <v>2822</v>
       </c>
       <c r="C8" t="s">
-        <v>2908</v>
+        <v>2906</v>
       </c>
       <c r="D8" t="s">
-        <v>2888</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -21811,13 +21825,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
+        <v>2915</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>2916</v>
+      </c>
+      <c r="D9" t="s">
         <v>2917</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>2918</v>
-      </c>
-      <c r="D9" t="s">
-        <v>2919</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -21825,13 +21839,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>2918</v>
+      </c>
+      <c r="C10" t="s">
         <v>2920</v>
       </c>
-      <c r="C10" t="s">
-        <v>2922</v>
-      </c>
       <c r="D10" t="s">
-        <v>2921</v>
+        <v>2919</v>
       </c>
     </row>
   </sheetData>
@@ -21857,10 +21871,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2715</v>
@@ -21874,13 +21888,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2832</v>
+        <v>2830</v>
       </c>
       <c r="C2" t="s">
         <v>2755</v>
       </c>
       <c r="D2" t="s">
-        <v>2892</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -21888,13 +21902,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2827</v>
+        <v>2825</v>
       </c>
       <c r="C3" t="s">
-        <v>2907</v>
+        <v>2905</v>
       </c>
       <c r="D3" t="s">
-        <v>2889</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21902,13 +21916,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2828</v>
+        <v>2826</v>
       </c>
       <c r="C4" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="D4" t="s">
-        <v>2890</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -21916,13 +21930,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2829</v>
+        <v>2827</v>
       </c>
       <c r="C5" t="s">
-        <v>2910</v>
+        <v>2908</v>
       </c>
       <c r="D5" t="s">
-        <v>2891</v>
+        <v>2889</v>
       </c>
     </row>
   </sheetData>
@@ -21953,10 +21967,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2807</v>
+        <v>2805</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2715</v>
@@ -21970,13 +21984,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>2871</v>
+        <v>2869</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>2755</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>2875</v>
+        <v>2873</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="26" customFormat="1">
@@ -21984,13 +21998,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>2755</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>2872</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -21998,13 +22012,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2830</v>
+        <v>2828</v>
       </c>
       <c r="C4" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="D4" t="s">
-        <v>2873</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -22012,13 +22026,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2831</v>
+        <v>2829</v>
       </c>
       <c r="C5" t="s">
-        <v>2909</v>
+        <v>2907</v>
       </c>
       <c r="D5" t="s">
-        <v>2874</v>
+        <v>2872</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="26" customFormat="1">
@@ -22026,13 +22040,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>2849</v>
+        <v>2847</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>2911</v>
+        <v>2909</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>2876</v>
+        <v>2874</v>
       </c>
     </row>
   </sheetData>
@@ -22048,10 +22062,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22065,10 +22079,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>2906</v>
+        <v>2904</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2792</v>
@@ -22083,10 +22097,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="C2" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>522</v>
@@ -22097,10 +22111,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="C3" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>523</v>
@@ -22111,10 +22125,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="C4" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>524</v>
@@ -22125,13 +22139,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>2865</v>
+        <v>2863</v>
       </c>
       <c r="C5" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>2869</v>
+        <v>2867</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -22139,10 +22153,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="C6" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>526</v>
@@ -22153,13 +22167,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>2866</v>
+        <v>2864</v>
       </c>
       <c r="C7" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>2806</v>
+        <v>2804</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -22167,10 +22181,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>2793</v>
+        <v>2863</v>
       </c>
       <c r="C8" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>571</v>
@@ -22182,10 +22196,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="C9" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>522</v>
@@ -22196,10 +22210,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="C10" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>523</v>
@@ -22210,10 +22224,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="C11" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>524</v>
@@ -22224,10 +22238,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2867</v>
+        <v>2865</v>
       </c>
       <c r="C12" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>525</v>
@@ -22238,13 +22252,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="C13" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="D13" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
       <c r="F13" s="20"/>
     </row>
@@ -22253,13 +22267,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="C14" t="s">
-        <v>2868</v>
+        <v>2866</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>2798</v>
+        <v>2796</v>
       </c>
       <c r="F14" s="16"/>
     </row>
@@ -22268,13 +22282,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>2870</v>
+        <v>2868</v>
       </c>
       <c r="C15" t="s">
-        <v>2795</v>
+        <v>2940</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>2796</v>
+        <v>2794</v>
       </c>
       <c r="F15" s="16"/>
     </row>
@@ -22283,13 +22297,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="C16" t="s">
-        <v>2799</v>
+        <v>2797</v>
       </c>
       <c r="D16" t="s">
-        <v>2797</v>
+        <v>2795</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -22297,13 +22311,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="C17" t="s">
-        <v>2800</v>
+        <v>2798</v>
       </c>
       <c r="D17" t="s">
-        <v>2801</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -22311,13 +22325,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>2794</v>
+        <v>2793</v>
       </c>
       <c r="C18" t="s">
-        <v>2802</v>
+        <v>2800</v>
       </c>
       <c r="D18" t="s">
-        <v>2803</v>
+        <v>2801</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -22334,11 +22348,103 @@
         <v>527</v>
       </c>
     </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>522</v>
+      </c>
+    </row>
     <row r="21" spans="1:4">
-      <c r="D21" s="19"/>
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="D22" s="19"/>
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>2867</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2864</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2864</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>2804</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2863</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2941</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>571</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adjustment to be able to upload also roxas vessels and a couple fo corrections
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3162" uniqueCount="2942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="2942">
   <si>
     <t>Afganistan</t>
   </si>
@@ -9091,12 +9091,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="145">
+  <cellStyleXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9284,7 +9286,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="145">
+  <cellStyles count="147">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -9428,6 +9430,8 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -22062,9 +22066,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -22446,6 +22450,20 @@
         <v>571</v>
       </c>
     </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2866</v>
+      </c>
+      <c r="D27" t="s">
+        <v>523</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
- summary year in the function - speed up the check_append for cell - swich for the reading txt files
</commit_message>
<xml_diff>
--- a/db_create/xcell_fk_tables.xlsx
+++ b/db_create/xcell_fk_tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="815" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="1540" yWindow="720" windowWidth="25600" windowHeight="16060" tabRatio="815" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="country_fk" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3685" uniqueCount="2958">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3688" uniqueCount="2960">
   <si>
     <t>Afganistan</t>
   </si>
@@ -8992,6 +8992,12 @@
   </si>
   <si>
     <t>NIH image</t>
+  </si>
+  <si>
+    <t>n_obs</t>
+  </si>
+  <si>
+    <t>number of observation (e.g.; number of cells in the ring)</t>
   </si>
 </sst>
 </file>
@@ -12440,10 +12446,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13149,6 +13155,20 @@
       </c>
       <c r="D50" s="14" t="s">
         <v>2743</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>2958</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2755</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>2959</v>
       </c>
     </row>
   </sheetData>
@@ -23669,7 +23689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A36" sqref="A36:XFD37"/>
     </sheetView>
   </sheetViews>

</xml_diff>